<commit_message>
fixed comparison counter in KMP
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Batur\HSE\Algorithms_3_cource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\Algorithms_3_cource\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B347CFC-929E-41C1-BCB0-6E312DDA55BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7900"/>
+    <workbookView xWindow="6888" yWindow="912" windowWidth="16224" windowHeight="10224" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -152,7 +153,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -339,30 +340,12 @@
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -383,6 +366,24 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -662,397 +663,397 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.26953125" customWidth="1"/>
-    <col min="4" max="4" width="22.08984375" customWidth="1"/>
-    <col min="5" max="5" width="22.1796875" customWidth="1"/>
-    <col min="6" max="6" width="22.7265625" customWidth="1"/>
-    <col min="7" max="7" width="21.7265625" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.21875" customWidth="1"/>
+    <col min="6" max="6" width="22.77734375" customWidth="1"/>
+    <col min="7" max="7" width="21.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30"/>
+    </row>
+    <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B5" s="9" t="s">
+      <c r="C4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="20" t="s">
+      <c r="D5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B6" s="9" t="s">
+      <c r="F5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B7" s="9" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B8" s="9" t="s">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="20" t="s">
+      <c r="C8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="21" t="s">
+      <c r="E8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="9" t="s">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="20" t="s">
+      <c r="C9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="20" t="s">
+      <c r="E9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="20" t="s">
+      <c r="E10" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="10" t="s">
+    <row r="11" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="23" t="s">
+      <c r="E11" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="G11" s="18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="11" t="s">
+    <row r="13" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="33"/>
+    </row>
+    <row r="15" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B16" s="14" t="s">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="25">
+      <c r="C16" s="19">
         <v>18</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="20">
         <v>9</v>
       </c>
-      <c r="E16" s="26">
+      <c r="E16" s="20">
         <v>10</v>
       </c>
-      <c r="F16" s="26">
-        <v>44</v>
-      </c>
-      <c r="G16" s="27">
+      <c r="F16" s="20">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="14" t="s">
+      <c r="G16" s="21">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="28">
+      <c r="C17" s="22">
         <v>910</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="23">
         <v>91</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="23">
         <v>100</v>
       </c>
-      <c r="F17" s="29">
-        <v>486</v>
-      </c>
-      <c r="G17" s="30">
+      <c r="F17" s="23">
         <v>190</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B18" s="14" t="s">
+      <c r="G17" s="24">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="28">
+      <c r="C18" s="22">
         <v>90100</v>
       </c>
-      <c r="D18" s="29">
+      <c r="D18" s="23">
         <v>901</v>
       </c>
-      <c r="E18" s="29">
+      <c r="E18" s="23">
         <v>1000</v>
       </c>
-      <c r="F18" s="29">
-        <v>4896</v>
-      </c>
-      <c r="G18" s="30">
+      <c r="F18" s="23">
         <v>1900</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B19" s="14" t="s">
+      <c r="G18" s="24">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="28">
+      <c r="C19" s="22">
         <v>4001000</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="23">
         <v>4001</v>
       </c>
-      <c r="E19" s="29">
+      <c r="E19" s="23">
         <v>5000</v>
       </c>
-      <c r="F19" s="29">
-        <v>23996</v>
-      </c>
-      <c r="G19" s="30">
+      <c r="F19" s="23">
         <v>9000</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B20" s="14" t="s">
+      <c r="G19" s="24">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="28">
+      <c r="C20" s="22">
         <v>633</v>
       </c>
-      <c r="D20" s="29">
+      <c r="D20" s="23">
         <v>600</v>
       </c>
-      <c r="E20" s="29">
+      <c r="E20" s="23">
         <v>67</v>
       </c>
-      <c r="F20" s="29">
-        <v>2019</v>
-      </c>
-      <c r="G20" s="30">
+      <c r="F20" s="23">
+        <v>633</v>
+      </c>
+      <c r="G20" s="24">
         <v>713</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B21" s="14" t="s">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="28">
+      <c r="C21" s="22">
         <v>695</v>
       </c>
-      <c r="D21" s="29">
+      <c r="D21" s="23">
         <v>611</v>
       </c>
-      <c r="E21" s="29">
+      <c r="E21" s="23">
         <v>106</v>
       </c>
-      <c r="F21" s="29">
-        <v>3011</v>
-      </c>
-      <c r="G21" s="30">
+      <c r="F21" s="23">
+        <v>695</v>
+      </c>
+      <c r="G21" s="24">
         <v>1158</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B22" s="14" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="28">
+      <c r="C22" s="22">
         <v>2074</v>
       </c>
-      <c r="D22" s="29">
+      <c r="D22" s="23">
         <v>1630</v>
       </c>
-      <c r="E22" s="29">
+      <c r="E22" s="23">
         <v>428</v>
       </c>
-      <c r="F22" s="29">
-        <v>9508</v>
-      </c>
-      <c r="G22" s="30">
+      <c r="F22" s="23">
+        <v>2070</v>
+      </c>
+      <c r="G22" s="24">
         <v>3539</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="15" t="s">
+    <row r="23" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="31">
+      <c r="C23" s="25">
         <v>9614</v>
       </c>
-      <c r="D23" s="32">
+      <c r="D23" s="26">
         <v>9523</v>
       </c>
-      <c r="E23" s="32">
+      <c r="E23" s="26">
         <v>499</v>
       </c>
-      <c r="F23" s="32">
-        <v>32800</v>
-      </c>
-      <c r="G23" s="33">
+      <c r="F23" s="26">
+        <v>9614</v>
+      </c>
+      <c r="G23" s="27">
         <v>10714</v>
       </c>
     </row>

</xml_diff>